<commit_message>
Add all helper method for the excel report.
</commit_message>
<xml_diff>
--- a/wwwroot/report.xlsx
+++ b/wwwroot/report.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
   <si>
     <t>Seal</t>
   </si>
@@ -48,7 +48,7 @@
     <t>STANBIC DAILY CASH OPERATION REPORT (NGN)</t>
   </si>
   <si>
-    <t>3/19/2020 9:49:50 AM</t>
+    <t>3/19/2020 11:11:27 AM</t>
   </si>
   <si>
     <t>1,000</t>
@@ -346,6 +346,204 @@
   </si>
   <si>
     <t>COUNTERFEITS (Pcs)</t>
+  </si>
+  <si>
+    <t>DATE OF PROCESSING</t>
+  </si>
+  <si>
+    <t>BANK NAME</t>
+  </si>
+  <si>
+    <t>Sterling Bank Plc</t>
+  </si>
+  <si>
+    <t>DATE OF DEPOSIT</t>
+  </si>
+  <si>
+    <t>BRIEF SUMMARY</t>
+  </si>
+  <si>
+    <t>Report Date:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3/19/2020 11:11:27 AM</t>
+  </si>
+  <si>
+    <t>Deposit Date:</t>
+  </si>
+  <si>
+    <t>Deposit Bank:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Heritage Banking Company Ltd</t>
+  </si>
+  <si>
+    <t>Decleared Value:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ₦200000000</t>
+  </si>
+  <si>
+    <t>Denominations:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1000: ₦15,000 500: ₦5,000,000 </t>
+  </si>
+  <si>
+    <t>PROCESSING DETAILS</t>
+  </si>
+  <si>
+    <t>BW Audit Trail</t>
+  </si>
+  <si>
+    <t>170619B1346411</t>
+  </si>
+  <si>
+    <t>Processing Date</t>
+  </si>
+  <si>
+    <t>3/19/2020 11:11:27 AM - 3/19/2020 11:11:27 AM</t>
+  </si>
+  <si>
+    <t>Bank Representative Witness</t>
+  </si>
+  <si>
+    <t>K. abayomi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment :  </t>
+  </si>
+  <si>
+    <t>SORTING SUMMARY</t>
+  </si>
+  <si>
+    <t>₦20,000,000</t>
+  </si>
+  <si>
+    <t>Post Sorting Value:</t>
+  </si>
+  <si>
+    <t>Shortages:</t>
+  </si>
+  <si>
+    <t>₦0</t>
+  </si>
+  <si>
+    <t>Overages:</t>
+  </si>
+  <si>
+    <t>Counterfeits:</t>
+  </si>
+  <si>
+    <t>Mix-ups:</t>
+  </si>
+  <si>
+    <t>DAILY TRANSACTIONS LOCAL CURRENCY (NGN)</t>
+  </si>
+  <si>
+    <t>#1000</t>
+  </si>
+  <si>
+    <t>#500</t>
+  </si>
+  <si>
+    <t>#200</t>
+  </si>
+  <si>
+    <t>#100</t>
+  </si>
+  <si>
+    <t>#50</t>
+  </si>
+  <si>
+    <t>#20</t>
+  </si>
+  <si>
+    <t>#10</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>BANK OPENNING BALANCE</t>
+  </si>
+  <si>
+    <t>599,679,000</t>
+  </si>
+  <si>
+    <t>502,852,000</t>
+  </si>
+  <si>
+    <t>3,505,400</t>
+  </si>
+  <si>
+    <t>2,406,800</t>
+  </si>
+  <si>
+    <t>259,250</t>
+  </si>
+  <si>
+    <t>501,540</t>
+  </si>
+  <si>
+    <t>43,960</t>
+  </si>
+  <si>
+    <t>48,510</t>
+  </si>
+  <si>
+    <t>1,109,296,460</t>
+  </si>
+  <si>
+    <t>INFLOW/EVACUATION</t>
+  </si>
+  <si>
+    <t>OYINGBO</t>
+  </si>
+  <si>
+    <t>AWOLOWO</t>
+  </si>
+  <si>
+    <t>Mutilated Evacuation</t>
+  </si>
+  <si>
+    <t>Evacuation in BW Wrapper</t>
+  </si>
+  <si>
+    <t>Evacuation in PAPER NOTE</t>
+  </si>
+  <si>
+    <t>TO BE RETURNED TO BRANCH</t>
+  </si>
+  <si>
+    <t>RETURNED TO VAULT</t>
+  </si>
+  <si>
+    <t>CASH SWAP</t>
+  </si>
+  <si>
+    <t>OTHERS:</t>
+  </si>
+  <si>
+    <t>TRANSFER FROM ILUPEJU</t>
+  </si>
+  <si>
+    <t>GUARANTY TRUST BANK PLC ILUPEJU CASH CENTER</t>
+  </si>
+  <si>
+    <t>At COB</t>
+  </si>
+  <si>
+    <t>GUARANTY TRUST BANK PLC ISLAND CASH CENTER</t>
+  </si>
+  <si>
+    <t>GUARANTY TRUST BANK PLC BOTH CASH CENTER</t>
   </si>
 </sst>
 </file>
@@ -353,7 +551,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -379,8 +577,13 @@
       <sz val="15"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000" tint="0"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,6 +593,21 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00008B" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF" tint="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -405,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
@@ -418,6 +636,18 @@
     <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="3" applyFill="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="3" applyFill="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="5" applyFill="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +658,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A2:Z42"/>
+  <dimension ref="A2:Z133"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1601,6 +1831,1581 @@
         <v>107</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" ht="40" customHeight="1">
+      <c r="A52" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="H53" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H54" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H56" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H57" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" ht="40" customHeight="1">
+      <c r="A61" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="G62" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" ht="40" customHeight="1">
+      <c r="A69" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="I70" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="I71" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="I72" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="I73" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="I74" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="I75" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B80" s="11"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="11"/>
+      <c r="J80" s="11"/>
+      <c r="K80" s="11"/>
+      <c r="L80" s="11"/>
+      <c r="M80" s="11"/>
+      <c r="N80" s="11"/>
+      <c r="O80" s="11"/>
+      <c r="P80" s="11"/>
+      <c r="Q80" s="11"/>
+      <c r="R80" s="11"/>
+      <c r="S80" s="11"/>
+      <c r="T80" s="11"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G81" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="H81" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="I81" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="J81" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="K81" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="L81" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="M81" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="N81" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="O81" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="P81" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q81" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="R81" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="S81" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B82" s="12"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="F82" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="G82" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="H82" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="I82" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="J82" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="K82" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="L82" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="M82" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="N82" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="O82" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="P82" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q82" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="R82" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="S82" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="T82" s="12"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10"/>
+      <c r="G83" s="10"/>
+      <c r="H83" s="10"/>
+      <c r="I83" s="10"/>
+      <c r="J83" s="10"/>
+      <c r="K83" s="10"/>
+      <c r="L83" s="10"/>
+      <c r="M83" s="10"/>
+      <c r="N83" s="10"/>
+      <c r="O83" s="10"/>
+      <c r="P83" s="10"/>
+      <c r="Q83" s="10"/>
+      <c r="R83" s="10"/>
+      <c r="S83" s="10"/>
+      <c r="T83" s="10"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E84" s="0">
+        <v>0</v>
+      </c>
+      <c r="F84" s="0">
+        <v>0</v>
+      </c>
+      <c r="G84" s="0">
+        <v>0</v>
+      </c>
+      <c r="H84" s="0">
+        <v>0</v>
+      </c>
+      <c r="I84" s="0">
+        <v>0</v>
+      </c>
+      <c r="J84" s="0">
+        <v>0</v>
+      </c>
+      <c r="K84" s="0">
+        <v>0</v>
+      </c>
+      <c r="L84" s="0">
+        <v>0</v>
+      </c>
+      <c r="M84" s="0">
+        <v>0</v>
+      </c>
+      <c r="N84" s="0">
+        <v>0</v>
+      </c>
+      <c r="O84" s="0">
+        <v>0</v>
+      </c>
+      <c r="P84" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q84" s="0">
+        <v>0</v>
+      </c>
+      <c r="R84" s="0">
+        <v>0</v>
+      </c>
+      <c r="S84" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="E85" s="0">
+        <v>0</v>
+      </c>
+      <c r="F85" s="0">
+        <v>0</v>
+      </c>
+      <c r="G85" s="0">
+        <v>0</v>
+      </c>
+      <c r="H85" s="0">
+        <v>0</v>
+      </c>
+      <c r="I85" s="0">
+        <v>0</v>
+      </c>
+      <c r="J85" s="0">
+        <v>0</v>
+      </c>
+      <c r="K85" s="0">
+        <v>0</v>
+      </c>
+      <c r="L85" s="0">
+        <v>0</v>
+      </c>
+      <c r="M85" s="0">
+        <v>0</v>
+      </c>
+      <c r="N85" s="0">
+        <v>0</v>
+      </c>
+      <c r="O85" s="0">
+        <v>0</v>
+      </c>
+      <c r="P85" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q85" s="0">
+        <v>0</v>
+      </c>
+      <c r="R85" s="0">
+        <v>0</v>
+      </c>
+      <c r="S85" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="E86" s="0">
+        <v>0</v>
+      </c>
+      <c r="F86" s="0">
+        <v>0</v>
+      </c>
+      <c r="G86" s="0">
+        <v>0</v>
+      </c>
+      <c r="H86" s="0">
+        <v>0</v>
+      </c>
+      <c r="I86" s="0">
+        <v>0</v>
+      </c>
+      <c r="J86" s="0">
+        <v>0</v>
+      </c>
+      <c r="K86" s="0">
+        <v>0</v>
+      </c>
+      <c r="L86" s="0">
+        <v>0</v>
+      </c>
+      <c r="M86" s="0">
+        <v>0</v>
+      </c>
+      <c r="N86" s="0">
+        <v>0</v>
+      </c>
+      <c r="O86" s="0">
+        <v>0</v>
+      </c>
+      <c r="P86" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q86" s="0">
+        <v>0</v>
+      </c>
+      <c r="R86" s="0">
+        <v>0</v>
+      </c>
+      <c r="S86" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B99" s="10"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B100" s="10"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
+    </row>
+    <row r="105" ht="40" customHeight="1">
+      <c r="A105" s="13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="6"/>
+      <c r="B106" s="6"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G106" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H106" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I106" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J106" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K106" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L106" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M106" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N106" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O106" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P106" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q106" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R106" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S106" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T106" s="6"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E107" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F107" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G107" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H107" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="I107" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="J107" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="K107" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="L107" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M107" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N107" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O107" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P107" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q107" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R107" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S107" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E108" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F108" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G108" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H108" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="I108" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J108" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="K108" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="L108" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="M108" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N108" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O108" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P108" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q108" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R108" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S108" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E109" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F109" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G109" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H109" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I109" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J109" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="K109" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="L109" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="M109" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N109" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O109" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P109" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q109" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R109" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S109" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E110" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F110" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="G110" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="H110" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="I110" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="J110" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="K110" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="L110" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="M110" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N110" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O110" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P110" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q110" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R110" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S110" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E111" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F111" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G111" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H111" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="I111" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J111" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="K111" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="L111" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="M111" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N111" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O111" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P111" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q111" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R111" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S111" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="E112" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F112" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G112" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="H112" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="I112" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="J112" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="K112" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="L112" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="M112" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N112" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O112" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P112" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q112" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R112" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S112" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="115" ht="40" customHeight="1">
+      <c r="A115" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="6"/>
+      <c r="B116" s="6"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F116" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G116" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H116" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I116" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J116" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K116" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L116" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M116" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N116" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O116" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P116" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q116" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R116" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S116" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T116" s="6"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E117" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F117" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G117" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H117" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="I117" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="J117" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="K117" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="L117" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M117" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N117" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O117" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P117" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q117" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R117" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S117" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E118" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F118" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G118" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H118" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="I118" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J118" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="K118" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="L118" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="M118" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N118" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O118" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P118" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q118" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R118" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S118" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F119" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G119" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H119" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I119" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J119" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="K119" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="L119" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="M119" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N119" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O119" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P119" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q119" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R119" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S119" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E120" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F120" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="G120" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="H120" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="I120" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="J120" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="K120" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="L120" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="M120" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N120" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O120" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P120" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q120" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R120" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S120" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E121" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F121" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G121" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H121" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="I121" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J121" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="K121" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="L121" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="M121" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N121" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O121" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P121" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q121" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R121" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S121" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="E122" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F122" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G122" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="H122" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="I122" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="J122" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="K122" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="L122" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="M122" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N122" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O122" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P122" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q122" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R122" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S122" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="126" ht="40" customHeight="1">
+      <c r="A126" s="13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="6"/>
+      <c r="B127" s="6"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="6"/>
+      <c r="E127" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F127" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G127" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H127" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I127" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J127" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K127" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L127" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M127" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N127" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O127" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P127" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q127" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R127" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S127" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T127" s="6"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E128" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F128" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G128" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H128" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="I128" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="J128" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="K128" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="L128" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M128" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N128" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O128" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P128" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q128" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R128" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S128" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E129" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F129" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G129" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H129" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="I129" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J129" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="K129" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="L129" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="M129" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N129" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O129" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P129" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q129" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R129" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S129" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E130" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F130" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G130" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H130" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I130" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J130" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="K130" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="L130" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="M130" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N130" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O130" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P130" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q130" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R130" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S130" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E131" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F131" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="G131" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="H131" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="I131" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="J131" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="K131" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="L131" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="M131" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N131" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O131" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P131" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q131" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R131" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S131" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E132" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F132" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G132" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H132" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="I132" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J132" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="K132" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="L132" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="M132" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N132" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O132" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P132" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q132" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R132" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S132" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="E133" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F133" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G133" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="H133" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="I133" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="J133" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="K133" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="L133" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="M133" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N133" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O133" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P133" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q133" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="R133" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="S133" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="B2:C2"/>
@@ -1613,7 +3418,7 @@
     <mergeCell ref="D3:E7"/>
     <mergeCell ref="F3:G7"/>
     <mergeCell ref="H3:I7"/>
-    <mergeCell ref="A9:O11"/>
+    <mergeCell ref="A9:T11"/>
     <mergeCell ref="A12:T12"/>
     <mergeCell ref="A13:T13"/>
     <mergeCell ref="A14:T14"/>
@@ -1633,7 +3438,7 @@
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:O34"/>
+    <mergeCell ref="A32:T34"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="A37:O37"/>
@@ -1642,6 +3447,89 @@
     <mergeCell ref="A40:C40"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A43:T45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="A49:T51"/>
+    <mergeCell ref="A52:O52"/>
+    <mergeCell ref="A53:G53"/>
+    <mergeCell ref="H53:O53"/>
+    <mergeCell ref="A54:G54"/>
+    <mergeCell ref="H54:O54"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="H55:O55"/>
+    <mergeCell ref="A56:G56"/>
+    <mergeCell ref="H56:O56"/>
+    <mergeCell ref="A57:G57"/>
+    <mergeCell ref="H57:O57"/>
+    <mergeCell ref="A58:T60"/>
+    <mergeCell ref="A61:O61"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="G62:O62"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="G63:O63"/>
+    <mergeCell ref="A64:F64"/>
+    <mergeCell ref="G64:O64"/>
+    <mergeCell ref="A65:O65"/>
+    <mergeCell ref="A66:T68"/>
+    <mergeCell ref="A69:O69"/>
+    <mergeCell ref="A70:H70"/>
+    <mergeCell ref="I70:O70"/>
+    <mergeCell ref="A71:H71"/>
+    <mergeCell ref="I71:O71"/>
+    <mergeCell ref="A72:H72"/>
+    <mergeCell ref="I72:O72"/>
+    <mergeCell ref="A73:H73"/>
+    <mergeCell ref="I73:O73"/>
+    <mergeCell ref="A74:H74"/>
+    <mergeCell ref="I74:O74"/>
+    <mergeCell ref="A75:H75"/>
+    <mergeCell ref="I75:O75"/>
+    <mergeCell ref="A77:T79"/>
+    <mergeCell ref="A80:T80"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="A83:D83"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="E87:T87"/>
+    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A91:D91"/>
+    <mergeCell ref="A93:D93"/>
+    <mergeCell ref="A95:D95"/>
+    <mergeCell ref="A97:D97"/>
+    <mergeCell ref="A99:D99"/>
+    <mergeCell ref="A100:D100"/>
+    <mergeCell ref="A102:T104"/>
+    <mergeCell ref="A105:T105"/>
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A108:D108"/>
+    <mergeCell ref="A109:D109"/>
+    <mergeCell ref="A110:D110"/>
+    <mergeCell ref="A111:D111"/>
+    <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A113:T114"/>
+    <mergeCell ref="A115:T115"/>
+    <mergeCell ref="A117:D117"/>
+    <mergeCell ref="A118:D118"/>
+    <mergeCell ref="A119:D119"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A121:D121"/>
+    <mergeCell ref="A122:D122"/>
+    <mergeCell ref="A123:T125"/>
+    <mergeCell ref="A126:T126"/>
+    <mergeCell ref="A128:D128"/>
+    <mergeCell ref="A129:D129"/>
+    <mergeCell ref="A130:D130"/>
+    <mergeCell ref="A131:D131"/>
+    <mergeCell ref="A132:D132"/>
+    <mergeCell ref="A133:D133"/>
   </mergeCells>
   <headerFooter/>
 </worksheet>

</xml_diff>